<commit_message>
Fix output.xlsx bimode global and choice columns
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -605,16 +605,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>2048</v>
       </c>
       <c r="F6" t="n">
         <v>2048</v>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>2048</v>
+      </c>
       <c r="H6" t="n">
         <v>0.006709000000000742</v>
       </c>
@@ -636,16 +636,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
         <v>2048</v>
       </c>
       <c r="F7" t="n">
-        <v>4096</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
+        <v>2048</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4096</v>
+      </c>
       <c r="H7" t="n">
         <v>0.006647999999998433</v>
       </c>
@@ -667,16 +667,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>2048</v>
       </c>
       <c r="F8" t="n">
-        <v>8192</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
+        <v>2048</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8192</v>
+      </c>
       <c r="H8" t="n">
         <v>0.006553999999994176</v>
       </c>
@@ -698,16 +698,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="F9" t="n">
-        <v>2048</v>
-      </c>
-      <c r="G9" t="inlineStr"/>
+        <v>4096</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2048</v>
+      </c>
       <c r="H9" t="n">
         <v>0.006307000000006724</v>
       </c>
@@ -729,16 +729,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="F10" t="n">
         <v>4096</v>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>4096</v>
+      </c>
       <c r="H10" t="n">
         <v>0.006198999999995181</v>
       </c>
@@ -760,16 +760,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="F11" t="n">
-        <v>8192</v>
-      </c>
-      <c r="G11" t="inlineStr"/>
+        <v>4096</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8192</v>
+      </c>
       <c r="H11" t="n">
         <v>0.006131999999993809</v>
       </c>
@@ -791,16 +791,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="F12" t="n">
-        <v>2048</v>
-      </c>
-      <c r="G12" t="inlineStr"/>
+        <v>8192</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2048</v>
+      </c>
       <c r="H12" t="n">
         <v>0.005919000000005781</v>
       </c>
@@ -822,16 +822,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="F13" t="n">
-        <v>4096</v>
-      </c>
-      <c r="G13" t="inlineStr"/>
+        <v>8192</v>
+      </c>
+      <c r="G13" t="n">
+        <v>4096</v>
+      </c>
       <c r="H13" t="n">
         <v>0.005829000000005635</v>
       </c>
@@ -853,16 +853,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="F14" t="n">
         <v>8192</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>8192</v>
+      </c>
       <c r="H14" t="n">
         <v>0.005757000000002677</v>
       </c>
@@ -884,16 +884,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="F15" t="n">
         <v>2048</v>
       </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>2048</v>
+      </c>
       <c r="H15" t="n">
         <v>0.006207000000003404</v>
       </c>
@@ -915,16 +915,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="F16" t="n">
-        <v>4096</v>
-      </c>
-      <c r="G16" t="inlineStr"/>
+        <v>2048</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4096</v>
+      </c>
       <c r="H16" t="n">
         <v>0.006161000000005856</v>
       </c>
@@ -946,16 +946,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="F17" t="n">
-        <v>8192</v>
-      </c>
-      <c r="G17" t="inlineStr"/>
+        <v>2048</v>
+      </c>
+      <c r="G17" t="n">
+        <v>8192</v>
+      </c>
       <c r="H17" t="n">
         <v>0.006066000000004124</v>
       </c>
@@ -977,16 +977,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>4096</v>
       </c>
       <c r="F18" t="n">
-        <v>2048</v>
-      </c>
-      <c r="G18" t="inlineStr"/>
+        <v>4096</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2048</v>
+      </c>
       <c r="H18" t="n">
         <v>0.0058169999999933</v>
       </c>
@@ -1008,16 +1008,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D19" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
         <v>4096</v>
       </c>
       <c r="F19" t="n">
         <v>4096</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>4096</v>
+      </c>
       <c r="H19" t="n">
         <v>0.005740000000002965</v>
       </c>
@@ -1039,16 +1039,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
         <v>4096</v>
       </c>
       <c r="F20" t="n">
-        <v>8192</v>
-      </c>
-      <c r="G20" t="inlineStr"/>
+        <v>4096</v>
+      </c>
+      <c r="G20" t="n">
+        <v>8192</v>
+      </c>
       <c r="H20" t="n">
         <v>0.005668999999997482</v>
       </c>
@@ -1070,16 +1070,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="F21" t="n">
-        <v>2048</v>
-      </c>
-      <c r="G21" t="inlineStr"/>
+        <v>8192</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2048</v>
+      </c>
       <c r="H21" t="n">
         <v>0.005442000000002167</v>
       </c>
@@ -1101,16 +1101,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="F22" t="n">
-        <v>4096</v>
-      </c>
-      <c r="G22" t="inlineStr"/>
+        <v>8192</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4096</v>
+      </c>
       <c r="H22" t="n">
         <v>0.005375999999998271</v>
       </c>
@@ -1132,16 +1132,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="F23" t="n">
         <v>8192</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>8192</v>
+      </c>
       <c r="H23" t="n">
         <v>0.005300000000005411</v>
       </c>
@@ -1807,16 +1807,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D44" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D44" t="inlineStr"/>
       <c r="E44" t="n">
         <v>2048</v>
       </c>
       <c r="F44" t="n">
         <v>2048</v>
       </c>
-      <c r="G44" t="inlineStr"/>
+      <c r="G44" t="n">
+        <v>2048</v>
+      </c>
       <c r="H44" t="n">
         <v>0.001512000000005287</v>
       </c>
@@ -1838,16 +1838,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D45" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D45" t="inlineStr"/>
       <c r="E45" t="n">
         <v>2048</v>
       </c>
       <c r="F45" t="n">
-        <v>4096</v>
-      </c>
-      <c r="G45" t="inlineStr"/>
+        <v>2048</v>
+      </c>
+      <c r="G45" t="n">
+        <v>4096</v>
+      </c>
       <c r="H45" t="n">
         <v>0.001520999999996775</v>
       </c>
@@ -1869,16 +1869,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D46" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="n">
         <v>2048</v>
       </c>
       <c r="F46" t="n">
-        <v>8192</v>
-      </c>
-      <c r="G46" t="inlineStr"/>
+        <v>2048</v>
+      </c>
+      <c r="G46" t="n">
+        <v>8192</v>
+      </c>
       <c r="H46" t="n">
         <v>0.001520999999996775</v>
       </c>
@@ -1900,16 +1900,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D47" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="F47" t="n">
-        <v>2048</v>
-      </c>
-      <c r="G47" t="inlineStr"/>
+        <v>4096</v>
+      </c>
+      <c r="G47" t="n">
+        <v>2048</v>
+      </c>
       <c r="H47" t="n">
         <v>0.004334999999997535</v>
       </c>
@@ -1931,16 +1931,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D48" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D48" t="inlineStr"/>
       <c r="E48" t="n">
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="F48" t="n">
         <v>4096</v>
       </c>
-      <c r="G48" t="inlineStr"/>
+      <c r="G48" t="n">
+        <v>4096</v>
+      </c>
       <c r="H48" t="n">
         <v>0.004334999999997535</v>
       </c>
@@ -1962,16 +1962,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D49" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="F49" t="n">
-        <v>8192</v>
-      </c>
-      <c r="G49" t="inlineStr"/>
+        <v>4096</v>
+      </c>
+      <c r="G49" t="n">
+        <v>8192</v>
+      </c>
       <c r="H49" t="n">
         <v>0.004337000000006697</v>
       </c>
@@ -1993,16 +1993,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D50" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="F50" t="n">
-        <v>2048</v>
-      </c>
-      <c r="G50" t="inlineStr"/>
+        <v>8192</v>
+      </c>
+      <c r="G50" t="n">
+        <v>2048</v>
+      </c>
       <c r="H50" t="n">
         <v>0.004341999999994073</v>
       </c>
@@ -2024,16 +2024,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D51" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="F51" t="n">
-        <v>4096</v>
-      </c>
-      <c r="G51" t="inlineStr"/>
+        <v>8192</v>
+      </c>
+      <c r="G51" t="n">
+        <v>4096</v>
+      </c>
       <c r="H51" t="n">
         <v>0.004341999999994073</v>
       </c>
@@ -2055,16 +2055,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D52" t="n">
-        <v>2048</v>
-      </c>
+      <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="F52" t="n">
         <v>8192</v>
       </c>
-      <c r="G52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>8192</v>
+      </c>
       <c r="H52" t="n">
         <v>0.004343000000005759</v>
       </c>
@@ -2086,16 +2086,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D53" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="F53" t="n">
         <v>2048</v>
       </c>
-      <c r="G53" t="inlineStr"/>
+      <c r="G53" t="n">
+        <v>2048</v>
+      </c>
       <c r="H53" t="n">
         <v>0.001502000000002113</v>
       </c>
@@ -2117,16 +2117,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D54" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="F54" t="n">
-        <v>4096</v>
-      </c>
-      <c r="G54" t="inlineStr"/>
+        <v>2048</v>
+      </c>
+      <c r="G54" t="n">
+        <v>4096</v>
+      </c>
       <c r="H54" t="n">
         <v>0.001512000000005287</v>
       </c>
@@ -2148,16 +2148,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D55" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="F55" t="n">
-        <v>8192</v>
-      </c>
-      <c r="G55" t="inlineStr"/>
+        <v>2048</v>
+      </c>
+      <c r="G55" t="n">
+        <v>8192</v>
+      </c>
       <c r="H55" t="n">
         <v>0.001512000000005287</v>
       </c>
@@ -2179,16 +2179,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D56" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
         <v>4096</v>
       </c>
       <c r="F56" t="n">
-        <v>2048</v>
-      </c>
-      <c r="G56" t="inlineStr"/>
+        <v>4096</v>
+      </c>
+      <c r="G56" t="n">
+        <v>2048</v>
+      </c>
       <c r="H56" t="n">
         <v>0.004306999999997174</v>
       </c>
@@ -2210,16 +2210,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D57" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
         <v>4096</v>
       </c>
       <c r="F57" t="n">
         <v>4096</v>
       </c>
-      <c r="G57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>4096</v>
+      </c>
       <c r="H57" t="n">
         <v>0.004306999999997174</v>
       </c>
@@ -2241,16 +2241,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D58" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
         <v>4096</v>
       </c>
       <c r="F58" t="n">
-        <v>8192</v>
-      </c>
-      <c r="G58" t="inlineStr"/>
+        <v>4096</v>
+      </c>
+      <c r="G58" t="n">
+        <v>8192</v>
+      </c>
       <c r="H58" t="n">
         <v>0.004309000000006336</v>
       </c>
@@ -2272,16 +2272,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D59" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="F59" t="n">
-        <v>2048</v>
-      </c>
-      <c r="G59" t="inlineStr"/>
+        <v>8192</v>
+      </c>
+      <c r="G59" t="n">
+        <v>2048</v>
+      </c>
       <c r="H59" t="n">
         <v>0.004313999999993712</v>
       </c>
@@ -2303,16 +2303,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D60" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="F60" t="n">
-        <v>4096</v>
-      </c>
-      <c r="G60" t="inlineStr"/>
+        <v>8192</v>
+      </c>
+      <c r="G60" t="n">
+        <v>4096</v>
+      </c>
       <c r="H60" t="n">
         <v>0.004313999999993712</v>
       </c>
@@ -2334,16 +2334,16 @@
           <t>BiMode</t>
         </is>
       </c>
-      <c r="D61" t="n">
-        <v>4096</v>
-      </c>
+      <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="F61" t="n">
         <v>8192</v>
       </c>
-      <c r="G61" t="inlineStr"/>
+      <c r="G61" t="n">
+        <v>8192</v>
+      </c>
       <c r="H61" t="n">
         <v>0.004315000000005398</v>
       </c>

</xml_diff>